<commit_message>
Test Data EXcel Library
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\eclipse-workspace\Project_Batch20_AutomationTest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE975C5A-8D96-4DCD-B6BE-860352C2B256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64F26A6-654C-4539-9070-7EA00E5B2D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Test@gmail.com</t>
   </si>
   <si>
     <t>Test123</t>
+  </si>
+  <si>
+    <t>123456789</t>
   </si>
 </sst>
 </file>
@@ -75,9 +78,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -359,23 +363,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1234890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>